<commit_message>
Modificación formato de fechas
</commit_message>
<xml_diff>
--- a/Veslink.Business/Resources/reporttemplate.xlsx
+++ b/Veslink.Business/Resources/reporttemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollos\Veslink\Repos\ReportExport\Veslink.Business\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A23DB49-20E8-4531-B30D-977CC0D1969D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F7C5A8-65AD-4DD0-B45C-7B5470DE6FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2430" windowWidth="29040" windowHeight="15720" xr2:uid="{76A4AEB4-3F70-4DB7-959B-860846F9256F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{76A4AEB4-3F70-4DB7-959B-860846F9256F}"/>
   </bookViews>
   <sheets>
     <sheet name="Input Form" sheetId="1" r:id="rId1"/>
@@ -1071,15 +1071,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="hh:mm;@"/>
-    <numFmt numFmtId="167" formatCode="h:mm;@"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="hh:mm;@"/>
+    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="34" x14ac:knownFonts="1">
     <font>
@@ -2254,16 +2253,16 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="276">
+  <cellXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
@@ -2279,10 +2278,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2609,13 +2608,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="23" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="23" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2633,7 +2632,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2667,7 +2666,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="33" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="9" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2679,7 +2678,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="9" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="33" fillId="9" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -2694,13 +2693,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="33" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="11" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2712,7 +2711,7 @@
     <xf numFmtId="0" fontId="26" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="11" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="33" fillId="11" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="11" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2724,10 +2723,10 @@
     <xf numFmtId="0" fontId="26" fillId="11" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="11" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="33" fillId="11" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="170" fontId="26" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="26" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="11" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2739,35 +2738,238 @@
     <xf numFmtId="0" fontId="26" fillId="11" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="11" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="33" fillId="11" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="11" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2806,240 +3008,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3465,16 +3456,16 @@
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
-      <c r="H3" s="238" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="239"/>
-      <c r="J3" s="239"/>
-      <c r="K3" s="239"/>
-      <c r="L3" s="239"/>
-      <c r="M3" s="239"/>
-      <c r="N3" s="239"/>
-      <c r="O3" s="240"/>
+      <c r="H3" s="219" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="220"/>
+      <c r="J3" s="220"/>
+      <c r="K3" s="220"/>
+      <c r="L3" s="220"/>
+      <c r="M3" s="220"/>
+      <c r="N3" s="220"/>
+      <c r="O3" s="202"/>
       <c r="P3" s="17"/>
     </row>
     <row r="4" spans="2:20" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3486,16 +3477,16 @@
       <c r="E4" s="22"/>
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
-      <c r="H4" s="241" t="s">
+      <c r="H4" s="221" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="241"/>
-      <c r="J4" s="241"/>
-      <c r="K4" s="241"/>
-      <c r="L4" s="241"/>
-      <c r="M4" s="241"/>
-      <c r="N4" s="241"/>
-      <c r="O4" s="242"/>
+      <c r="I4" s="221"/>
+      <c r="J4" s="221"/>
+      <c r="K4" s="221"/>
+      <c r="L4" s="221"/>
+      <c r="M4" s="221"/>
+      <c r="N4" s="221"/>
+      <c r="O4" s="222"/>
       <c r="P4" s="17"/>
       <c r="T4" s="13" t="s">
         <v>170</v>
@@ -3512,16 +3503,16 @@
         <v>3</v>
       </c>
       <c r="G5" s="24"/>
-      <c r="H5" s="243" t="s">
+      <c r="H5" s="223" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="243"/>
-      <c r="J5" s="243"/>
-      <c r="K5" s="243"/>
-      <c r="L5" s="243"/>
-      <c r="M5" s="243"/>
-      <c r="N5" s="243"/>
-      <c r="O5" s="244"/>
+      <c r="I5" s="223"/>
+      <c r="J5" s="223"/>
+      <c r="K5" s="223"/>
+      <c r="L5" s="223"/>
+      <c r="M5" s="223"/>
+      <c r="N5" s="223"/>
+      <c r="O5" s="224"/>
       <c r="P5" s="17"/>
     </row>
     <row r="6" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3535,16 +3526,16 @@
         <v>5</v>
       </c>
       <c r="G6" s="19"/>
-      <c r="H6" s="245" t="s">
+      <c r="H6" s="225" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="245"/>
-      <c r="J6" s="245"/>
-      <c r="K6" s="245"/>
-      <c r="L6" s="245"/>
-      <c r="M6" s="245"/>
-      <c r="N6" s="245"/>
-      <c r="O6" s="246"/>
+      <c r="I6" s="225"/>
+      <c r="J6" s="225"/>
+      <c r="K6" s="225"/>
+      <c r="L6" s="225"/>
+      <c r="M6" s="225"/>
+      <c r="N6" s="225"/>
+      <c r="O6" s="226"/>
       <c r="P6" s="17"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
@@ -3600,8 +3591,8 @@
       <c r="E9" s="40">
         <v>2</v>
       </c>
-      <c r="F9" s="247"/>
-      <c r="G9" s="248"/>
+      <c r="F9" s="227"/>
+      <c r="G9" s="228"/>
       <c r="H9" s="41"/>
       <c r="I9" s="42" t="s">
         <v>12</v>
@@ -3624,8 +3615,8 @@
         <f>IF(F10&lt;&gt;"",2,0)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="232"/>
-      <c r="G10" s="233"/>
+      <c r="F10" s="187"/>
+      <c r="G10" s="188"/>
       <c r="H10" s="46"/>
       <c r="I10" s="47" t="s">
         <v>14</v>
@@ -3648,10 +3639,10 @@
         <f>IF(F11&lt;&gt;"",2,0)</f>
         <v>2</v>
       </c>
-      <c r="F11" s="232" t="s">
+      <c r="F11" s="187" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="233"/>
+      <c r="G11" s="188"/>
       <c r="H11" s="46"/>
       <c r="I11" s="47" t="s">
         <v>17</v>
@@ -3673,8 +3664,8 @@
       <c r="E12" s="29">
         <v>2</v>
       </c>
-      <c r="F12" s="236"/>
-      <c r="G12" s="237"/>
+      <c r="F12" s="215"/>
+      <c r="G12" s="216"/>
       <c r="H12" s="49" t="s">
         <v>19</v>
       </c>
@@ -3696,10 +3687,10 @@
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
       <c r="E13" s="52"/>
-      <c r="F13" s="249" t="s">
+      <c r="F13" s="217" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="250"/>
+      <c r="G13" s="218"/>
       <c r="H13" s="46"/>
       <c r="I13" s="47" t="s">
         <v>23</v>
@@ -3721,8 +3712,8 @@
       <c r="E14" s="29">
         <v>22</v>
       </c>
-      <c r="F14" s="251"/>
-      <c r="G14" s="252"/>
+      <c r="F14" s="211"/>
+      <c r="G14" s="212"/>
       <c r="H14" s="46"/>
       <c r="I14" s="47" t="s">
         <v>25</v>
@@ -3736,20 +3727,20 @@
       <c r="P14" s="17"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="253"/>
-      <c r="C15" s="254"/>
-      <c r="D15" s="254"/>
-      <c r="E15" s="254"/>
-      <c r="F15" s="254"/>
-      <c r="G15" s="255"/>
-      <c r="H15" s="255"/>
-      <c r="I15" s="255"/>
-      <c r="J15" s="255"/>
-      <c r="K15" s="255"/>
-      <c r="L15" s="255"/>
-      <c r="M15" s="255"/>
-      <c r="N15" s="255"/>
-      <c r="O15" s="240"/>
+      <c r="B15" s="199"/>
+      <c r="C15" s="200"/>
+      <c r="D15" s="200"/>
+      <c r="E15" s="200"/>
+      <c r="F15" s="200"/>
+      <c r="G15" s="201"/>
+      <c r="H15" s="201"/>
+      <c r="I15" s="201"/>
+      <c r="J15" s="201"/>
+      <c r="K15" s="201"/>
+      <c r="L15" s="201"/>
+      <c r="M15" s="201"/>
+      <c r="N15" s="201"/>
+      <c r="O15" s="202"/>
       <c r="P15" s="17"/>
     </row>
     <row r="16" spans="2:20" ht="18.75" x14ac:dyDescent="0.25">
@@ -3804,18 +3795,18 @@
         <f>IF(F18&lt;&gt;"",2,0)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="222"/>
-      <c r="G18" s="223"/>
+      <c r="F18" s="236"/>
+      <c r="G18" s="237"/>
       <c r="H18" s="41"/>
-      <c r="I18" s="224" t="s">
+      <c r="I18" s="238" t="s">
         <v>29</v>
       </c>
-      <c r="J18" s="224"/>
-      <c r="K18" s="224"/>
-      <c r="L18" s="224"/>
-      <c r="M18" s="224"/>
-      <c r="N18" s="224"/>
-      <c r="O18" s="225"/>
+      <c r="J18" s="238"/>
+      <c r="K18" s="238"/>
+      <c r="L18" s="238"/>
+      <c r="M18" s="238"/>
+      <c r="N18" s="238"/>
+      <c r="O18" s="239"/>
       <c r="P18" s="17"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -3828,8 +3819,8 @@
         <f>IF(F19&lt;&gt;"",IF(AND(LEN(F19)&gt;=S19,LEN(F19)&lt;=T19),2,1),0)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="251"/>
-      <c r="G19" s="252"/>
+      <c r="F19" s="211"/>
+      <c r="G19" s="212"/>
       <c r="H19" s="61"/>
       <c r="I19" s="62" t="s">
         <v>31</v>
@@ -3852,18 +3843,18 @@
         <f>IF(F20&lt;&gt;"",2,0)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="232"/>
-      <c r="G20" s="233"/>
+      <c r="F20" s="187"/>
+      <c r="G20" s="188"/>
       <c r="H20" s="46"/>
-      <c r="I20" s="214" t="s">
+      <c r="I20" s="213" t="s">
         <v>33</v>
       </c>
-      <c r="J20" s="214"/>
-      <c r="K20" s="214"/>
-      <c r="L20" s="214"/>
-      <c r="M20" s="214"/>
-      <c r="N20" s="214"/>
-      <c r="O20" s="215"/>
+      <c r="J20" s="213"/>
+      <c r="K20" s="213"/>
+      <c r="L20" s="213"/>
+      <c r="M20" s="213"/>
+      <c r="N20" s="213"/>
+      <c r="O20" s="214"/>
       <c r="P20" s="17"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -3876,8 +3867,8 @@
         <f>IF(F21&lt;&gt;"",IF(AND(LEN(F21)&gt;=S21,LEN(F21)&lt;=T21),2,1),0)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="251"/>
-      <c r="G21" s="252"/>
+      <c r="F21" s="211"/>
+      <c r="G21" s="212"/>
       <c r="H21" s="46"/>
       <c r="I21" s="62" t="s">
         <v>34</v>
@@ -3899,21 +3890,21 @@
       <c r="E22" s="29">
         <v>2</v>
       </c>
-      <c r="F22" s="226"/>
-      <c r="G22" s="227"/>
+      <c r="F22" s="187"/>
+      <c r="G22" s="188"/>
       <c r="H22" s="49" t="str">
         <f>T4</f>
         <v>DD-MM-YYYY</v>
       </c>
-      <c r="I22" s="228" t="s">
+      <c r="I22" s="195" t="s">
         <v>36</v>
       </c>
-      <c r="J22" s="228"/>
-      <c r="K22" s="228"/>
-      <c r="L22" s="228"/>
-      <c r="M22" s="228"/>
-      <c r="N22" s="228"/>
-      <c r="O22" s="229"/>
+      <c r="J22" s="195"/>
+      <c r="K22" s="195"/>
+      <c r="L22" s="195"/>
+      <c r="M22" s="195"/>
+      <c r="N22" s="195"/>
+      <c r="O22" s="196"/>
       <c r="P22" s="17"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
@@ -3925,18 +3916,18 @@
       <c r="E23" s="29">
         <v>2</v>
       </c>
-      <c r="F23" s="230"/>
-      <c r="G23" s="231"/>
+      <c r="F23" s="240"/>
+      <c r="G23" s="241"/>
       <c r="H23" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="I23" s="228"/>
-      <c r="J23" s="228"/>
-      <c r="K23" s="228"/>
-      <c r="L23" s="228"/>
-      <c r="M23" s="228"/>
-      <c r="N23" s="228"/>
-      <c r="O23" s="229"/>
+      <c r="I23" s="195"/>
+      <c r="J23" s="195"/>
+      <c r="K23" s="195"/>
+      <c r="L23" s="195"/>
+      <c r="M23" s="195"/>
+      <c r="N23" s="195"/>
+      <c r="O23" s="196"/>
       <c r="P23" s="17"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
@@ -3948,21 +3939,21 @@
       <c r="E24" s="29">
         <v>2</v>
       </c>
-      <c r="F24" s="226"/>
-      <c r="G24" s="227"/>
+      <c r="F24" s="187"/>
+      <c r="G24" s="188"/>
       <c r="H24" s="49" t="str">
         <f>H22</f>
         <v>DD-MM-YYYY</v>
       </c>
-      <c r="I24" s="228" t="s">
+      <c r="I24" s="195" t="s">
         <v>40</v>
       </c>
-      <c r="J24" s="228"/>
-      <c r="K24" s="228"/>
-      <c r="L24" s="228"/>
-      <c r="M24" s="228"/>
-      <c r="N24" s="228"/>
-      <c r="O24" s="229"/>
+      <c r="J24" s="195"/>
+      <c r="K24" s="195"/>
+      <c r="L24" s="195"/>
+      <c r="M24" s="195"/>
+      <c r="N24" s="195"/>
+      <c r="O24" s="196"/>
       <c r="P24" s="17"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
@@ -3974,18 +3965,18 @@
       <c r="E25" s="29">
         <v>2</v>
       </c>
-      <c r="F25" s="230"/>
-      <c r="G25" s="231"/>
+      <c r="F25" s="240"/>
+      <c r="G25" s="241"/>
       <c r="H25" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="228"/>
-      <c r="J25" s="228"/>
-      <c r="K25" s="228"/>
-      <c r="L25" s="228"/>
-      <c r="M25" s="228"/>
-      <c r="N25" s="228"/>
-      <c r="O25" s="229"/>
+      <c r="I25" s="195"/>
+      <c r="J25" s="195"/>
+      <c r="K25" s="195"/>
+      <c r="L25" s="195"/>
+      <c r="M25" s="195"/>
+      <c r="N25" s="195"/>
+      <c r="O25" s="196"/>
       <c r="P25" s="17"/>
     </row>
     <row r="26" spans="2:16" ht="30" x14ac:dyDescent="0.25">
@@ -3997,37 +3988,37 @@
       <c r="E26" s="29">
         <v>2</v>
       </c>
-      <c r="F26" s="236"/>
-      <c r="G26" s="237"/>
+      <c r="F26" s="215"/>
+      <c r="G26" s="216"/>
       <c r="H26" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="I26" s="214" t="s">
+      <c r="I26" s="213" t="s">
         <v>44</v>
       </c>
-      <c r="J26" s="214"/>
-      <c r="K26" s="214"/>
-      <c r="L26" s="214"/>
-      <c r="M26" s="214"/>
-      <c r="N26" s="214"/>
-      <c r="O26" s="215"/>
+      <c r="J26" s="213"/>
+      <c r="K26" s="213"/>
+      <c r="L26" s="213"/>
+      <c r="M26" s="213"/>
+      <c r="N26" s="213"/>
+      <c r="O26" s="214"/>
       <c r="P26" s="17"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="253"/>
-      <c r="C27" s="254"/>
-      <c r="D27" s="254"/>
-      <c r="E27" s="254"/>
-      <c r="F27" s="254"/>
-      <c r="G27" s="255"/>
-      <c r="H27" s="255"/>
-      <c r="I27" s="255"/>
-      <c r="J27" s="255"/>
-      <c r="K27" s="255"/>
-      <c r="L27" s="255"/>
-      <c r="M27" s="255"/>
-      <c r="N27" s="255"/>
-      <c r="O27" s="240"/>
+      <c r="B27" s="199"/>
+      <c r="C27" s="200"/>
+      <c r="D27" s="200"/>
+      <c r="E27" s="200"/>
+      <c r="F27" s="200"/>
+      <c r="G27" s="201"/>
+      <c r="H27" s="201"/>
+      <c r="I27" s="201"/>
+      <c r="J27" s="201"/>
+      <c r="K27" s="201"/>
+      <c r="L27" s="201"/>
+      <c r="M27" s="201"/>
+      <c r="N27" s="201"/>
+      <c r="O27" s="202"/>
       <c r="P27" s="17"/>
     </row>
     <row r="28" spans="2:16" ht="18.75" x14ac:dyDescent="0.25">
@@ -4059,15 +4050,15 @@
       <c r="H29" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="I29" s="256" t="s">
+      <c r="I29" s="203" t="s">
         <v>10</v>
       </c>
-      <c r="J29" s="256"/>
-      <c r="K29" s="256"/>
-      <c r="L29" s="256"/>
-      <c r="M29" s="256"/>
-      <c r="N29" s="256"/>
-      <c r="O29" s="257"/>
+      <c r="J29" s="203"/>
+      <c r="K29" s="203"/>
+      <c r="L29" s="203"/>
+      <c r="M29" s="203"/>
+      <c r="N29" s="203"/>
+      <c r="O29" s="204"/>
       <c r="P29" s="37"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
@@ -4077,21 +4068,21 @@
       <c r="C30" s="39"/>
       <c r="D30" s="39"/>
       <c r="E30" s="40"/>
-      <c r="F30" s="258" t="str">
+      <c r="F30" s="205" t="str">
         <f>F20&amp;""</f>
         <v/>
       </c>
-      <c r="G30" s="259"/>
+      <c r="G30" s="206"/>
       <c r="H30" s="41"/>
-      <c r="I30" s="260" t="s">
+      <c r="I30" s="207" t="s">
         <v>47</v>
       </c>
-      <c r="J30" s="260"/>
-      <c r="K30" s="260"/>
-      <c r="L30" s="260"/>
-      <c r="M30" s="260"/>
-      <c r="N30" s="260"/>
-      <c r="O30" s="261"/>
+      <c r="J30" s="207"/>
+      <c r="K30" s="207"/>
+      <c r="L30" s="207"/>
+      <c r="M30" s="207"/>
+      <c r="N30" s="207"/>
+      <c r="O30" s="208"/>
       <c r="P30" s="17"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
@@ -4101,21 +4092,21 @@
       <c r="C31" s="59"/>
       <c r="D31" s="60"/>
       <c r="E31" s="29"/>
-      <c r="F31" s="258" t="str">
+      <c r="F31" s="205" t="str">
         <f>F21&amp;""</f>
         <v/>
       </c>
-      <c r="G31" s="259"/>
+      <c r="G31" s="206"/>
       <c r="H31" s="61"/>
-      <c r="I31" s="262" t="s">
+      <c r="I31" s="209" t="s">
         <v>48</v>
       </c>
-      <c r="J31" s="262"/>
-      <c r="K31" s="262"/>
-      <c r="L31" s="262"/>
-      <c r="M31" s="262"/>
-      <c r="N31" s="262"/>
-      <c r="O31" s="263"/>
+      <c r="J31" s="209"/>
+      <c r="K31" s="209"/>
+      <c r="L31" s="209"/>
+      <c r="M31" s="209"/>
+      <c r="N31" s="209"/>
+      <c r="O31" s="210"/>
       <c r="P31" s="17"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
@@ -4128,18 +4119,18 @@
         <f>IF(F32&lt;&gt;"",2,0)</f>
         <v>0</v>
       </c>
-      <c r="F32" s="232"/>
-      <c r="G32" s="233"/>
+      <c r="F32" s="187"/>
+      <c r="G32" s="188"/>
       <c r="H32" s="46"/>
-      <c r="I32" s="234" t="s">
+      <c r="I32" s="242" t="s">
         <v>50</v>
       </c>
-      <c r="J32" s="234"/>
-      <c r="K32" s="234"/>
-      <c r="L32" s="234"/>
-      <c r="M32" s="234"/>
-      <c r="N32" s="234"/>
-      <c r="O32" s="235"/>
+      <c r="J32" s="242"/>
+      <c r="K32" s="242"/>
+      <c r="L32" s="242"/>
+      <c r="M32" s="242"/>
+      <c r="N32" s="242"/>
+      <c r="O32" s="243"/>
       <c r="P32" s="17"/>
     </row>
     <row r="33" spans="2:26" x14ac:dyDescent="0.25">
@@ -4152,8 +4143,8 @@
         <f>IF(F33&lt;&gt;"",IF(AND(LEN(F33)&gt;=S33,LEN(F33)&lt;=T33),2,1),0)</f>
         <v>0</v>
       </c>
-      <c r="F33" s="232"/>
-      <c r="G33" s="233"/>
+      <c r="F33" s="187"/>
+      <c r="G33" s="188"/>
       <c r="H33" s="46"/>
       <c r="I33" s="62" t="s">
         <v>51</v>
@@ -4175,21 +4166,21 @@
       <c r="E34" s="29">
         <v>2</v>
       </c>
-      <c r="F34" s="268"/>
-      <c r="G34" s="269"/>
+      <c r="F34" s="189"/>
+      <c r="G34" s="190"/>
       <c r="H34" s="49" t="str">
         <f>H22</f>
         <v>DD-MM-YYYY</v>
       </c>
-      <c r="I34" s="266" t="s">
+      <c r="I34" s="185" t="s">
         <v>53</v>
       </c>
-      <c r="J34" s="270"/>
-      <c r="K34" s="270"/>
-      <c r="L34" s="270"/>
-      <c r="M34" s="270"/>
-      <c r="N34" s="270"/>
-      <c r="O34" s="271"/>
+      <c r="J34" s="191"/>
+      <c r="K34" s="191"/>
+      <c r="L34" s="191"/>
+      <c r="M34" s="191"/>
+      <c r="N34" s="191"/>
+      <c r="O34" s="192"/>
       <c r="P34" s="17"/>
     </row>
     <row r="35" spans="2:26" x14ac:dyDescent="0.25">
@@ -4201,18 +4192,18 @@
       <c r="E35" s="29">
         <v>2</v>
       </c>
-      <c r="F35" s="272"/>
-      <c r="G35" s="273"/>
+      <c r="F35" s="193"/>
+      <c r="G35" s="194"/>
       <c r="H35" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="I35" s="270"/>
-      <c r="J35" s="270"/>
-      <c r="K35" s="270"/>
-      <c r="L35" s="270"/>
-      <c r="M35" s="270"/>
-      <c r="N35" s="270"/>
-      <c r="O35" s="271"/>
+      <c r="I35" s="191"/>
+      <c r="J35" s="191"/>
+      <c r="K35" s="191"/>
+      <c r="L35" s="191"/>
+      <c r="M35" s="191"/>
+      <c r="N35" s="191"/>
+      <c r="O35" s="192"/>
       <c r="P35" s="17"/>
     </row>
     <row r="36" spans="2:26" x14ac:dyDescent="0.25">
@@ -4224,21 +4215,21 @@
       <c r="E36" s="29">
         <v>2</v>
       </c>
-      <c r="F36" s="226"/>
-      <c r="G36" s="227"/>
+      <c r="F36" s="187"/>
+      <c r="G36" s="188"/>
       <c r="H36" s="49" t="str">
         <f>H22</f>
         <v>DD-MM-YYYY</v>
       </c>
-      <c r="I36" s="228" t="s">
+      <c r="I36" s="195" t="s">
         <v>56</v>
       </c>
-      <c r="J36" s="228"/>
-      <c r="K36" s="228"/>
-      <c r="L36" s="228"/>
-      <c r="M36" s="228"/>
-      <c r="N36" s="228"/>
-      <c r="O36" s="229"/>
+      <c r="J36" s="195"/>
+      <c r="K36" s="195"/>
+      <c r="L36" s="195"/>
+      <c r="M36" s="195"/>
+      <c r="N36" s="195"/>
+      <c r="O36" s="196"/>
       <c r="P36" s="17"/>
     </row>
     <row r="37" spans="2:26" x14ac:dyDescent="0.25">
@@ -4250,18 +4241,18 @@
       <c r="E37" s="29">
         <v>2</v>
       </c>
-      <c r="F37" s="274"/>
-      <c r="G37" s="275"/>
+      <c r="F37" s="197"/>
+      <c r="G37" s="198"/>
       <c r="H37" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="I37" s="228"/>
-      <c r="J37" s="228"/>
-      <c r="K37" s="228"/>
-      <c r="L37" s="228"/>
-      <c r="M37" s="228"/>
-      <c r="N37" s="228"/>
-      <c r="O37" s="229"/>
+      <c r="I37" s="195"/>
+      <c r="J37" s="195"/>
+      <c r="K37" s="195"/>
+      <c r="L37" s="195"/>
+      <c r="M37" s="195"/>
+      <c r="N37" s="195"/>
+      <c r="O37" s="196"/>
       <c r="P37" s="17"/>
     </row>
     <row r="38" spans="2:26" x14ac:dyDescent="0.25">
@@ -4273,23 +4264,23 @@
       <c r="E38" s="29">
         <v>2</v>
       </c>
-      <c r="F38" s="264" t="str">
+      <c r="F38" s="183" t="str">
         <f>IF(AND(ISBLANK(G46),ISBLANK(G48),ISBLANK(G50),ISBLANK(G52),ISBLANK(G54),ISBLANK(G56),ISBLANK(G58),ISBLANK(G60),ISBLANK(G62),ISBLANK(G64),ISBLANK(G66)),"",(SUM(G45:G67)))</f>
         <v/>
       </c>
-      <c r="G38" s="265"/>
+      <c r="G38" s="184"/>
       <c r="H38" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="I38" s="266" t="s">
+      <c r="I38" s="185" t="s">
         <v>59</v>
       </c>
-      <c r="J38" s="266"/>
-      <c r="K38" s="266"/>
-      <c r="L38" s="266"/>
-      <c r="M38" s="266"/>
-      <c r="N38" s="266"/>
-      <c r="O38" s="267"/>
+      <c r="J38" s="185"/>
+      <c r="K38" s="185"/>
+      <c r="L38" s="185"/>
+      <c r="M38" s="185"/>
+      <c r="N38" s="185"/>
+      <c r="O38" s="186"/>
       <c r="P38" s="17"/>
     </row>
     <row r="39" spans="2:26" x14ac:dyDescent="0.25"/>
@@ -4312,22 +4303,22 @@
       <c r="O40" s="55"/>
     </row>
     <row r="41" spans="2:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="213" t="s">
+      <c r="B41" s="229" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="214"/>
-      <c r="D41" s="214"/>
-      <c r="E41" s="214"/>
-      <c r="F41" s="214"/>
-      <c r="G41" s="214"/>
-      <c r="H41" s="214"/>
-      <c r="I41" s="214"/>
-      <c r="J41" s="214"/>
-      <c r="K41" s="214"/>
-      <c r="L41" s="214"/>
-      <c r="M41" s="214"/>
-      <c r="N41" s="214"/>
-      <c r="O41" s="215"/>
+      <c r="C41" s="213"/>
+      <c r="D41" s="213"/>
+      <c r="E41" s="213"/>
+      <c r="F41" s="213"/>
+      <c r="G41" s="213"/>
+      <c r="H41" s="213"/>
+      <c r="I41" s="213"/>
+      <c r="J41" s="213"/>
+      <c r="K41" s="213"/>
+      <c r="L41" s="213"/>
+      <c r="M41" s="213"/>
+      <c r="N41" s="213"/>
+      <c r="O41" s="214"/>
     </row>
     <row r="42" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B42" s="70"/>
@@ -4361,12 +4352,12 @@
       <c r="O42" s="75"/>
     </row>
     <row r="43" spans="2:26" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="216"/>
-      <c r="C43" s="217"/>
-      <c r="D43" s="218" t="s">
+      <c r="B43" s="230"/>
+      <c r="C43" s="231"/>
+      <c r="D43" s="232" t="s">
         <v>62</v>
       </c>
-      <c r="E43" s="219"/>
+      <c r="E43" s="233"/>
       <c r="F43" s="76" t="s">
         <v>63</v>
       </c>
@@ -4423,11 +4414,11 @@
         <v>72</v>
       </c>
       <c r="C44" s="29"/>
-      <c r="D44" s="220" t="str">
+      <c r="D44" s="234" t="str">
         <f>F18&amp;""</f>
         <v/>
       </c>
-      <c r="E44" s="221"/>
+      <c r="E44" s="235"/>
       <c r="F44" s="82" t="str">
         <f>F20&amp;""</f>
         <v/>
@@ -4465,15 +4456,15 @@
         <v>73</v>
       </c>
       <c r="C45" s="29"/>
-      <c r="D45" s="210" t="str">
+      <c r="D45" s="244" t="str">
         <f>F30&amp;""</f>
         <v/>
       </c>
-      <c r="E45" s="211"/>
-      <c r="F45" s="208" t="s">
+      <c r="E45" s="245"/>
+      <c r="F45" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="G45" s="209"/>
+      <c r="G45" s="247"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="2"/>
@@ -4512,8 +4503,8 @@
         <v>75</v>
       </c>
       <c r="C46" s="29"/>
-      <c r="D46" s="212"/>
-      <c r="E46" s="205"/>
+      <c r="D46" s="248"/>
+      <c r="E46" s="249"/>
       <c r="F46" s="5"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
@@ -4551,15 +4542,15 @@
         <v>76</v>
       </c>
       <c r="C47" s="29"/>
-      <c r="D47" s="206" t="str">
+      <c r="D47" s="250" t="str">
         <f>IF(F46="","_empty_",F46)</f>
         <v>_empty_</v>
       </c>
-      <c r="E47" s="207"/>
-      <c r="F47" s="208" t="s">
+      <c r="E47" s="251"/>
+      <c r="F47" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="G47" s="209"/>
+      <c r="G47" s="247"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="2"/>
@@ -4595,8 +4586,8 @@
         <v>77</v>
       </c>
       <c r="C48" s="29"/>
-      <c r="D48" s="204"/>
-      <c r="E48" s="205"/>
+      <c r="D48" s="252"/>
+      <c r="E48" s="249"/>
       <c r="F48" s="5"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
@@ -4634,15 +4625,15 @@
         <v>78</v>
       </c>
       <c r="C49" s="29"/>
-      <c r="D49" s="206" t="str">
+      <c r="D49" s="250" t="str">
         <f>IF(F48="","_empty_",F48)</f>
         <v>_empty_</v>
       </c>
-      <c r="E49" s="207"/>
-      <c r="F49" s="208" t="s">
+      <c r="E49" s="251"/>
+      <c r="F49" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="G49" s="209"/>
+      <c r="G49" s="247"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="2"/>
@@ -4678,8 +4669,8 @@
         <v>79</v>
       </c>
       <c r="C50" s="29"/>
-      <c r="D50" s="204"/>
-      <c r="E50" s="205"/>
+      <c r="D50" s="252"/>
+      <c r="E50" s="249"/>
       <c r="F50" s="6"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
@@ -4717,15 +4708,15 @@
         <v>80</v>
       </c>
       <c r="C51" s="29"/>
-      <c r="D51" s="206" t="str">
+      <c r="D51" s="250" t="str">
         <f>IF(F50="","_empty_",F50)</f>
         <v>_empty_</v>
       </c>
-      <c r="E51" s="207"/>
-      <c r="F51" s="208" t="s">
+      <c r="E51" s="251"/>
+      <c r="F51" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="G51" s="209"/>
+      <c r="G51" s="247"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="J51" s="2"/>
@@ -4761,8 +4752,8 @@
         <v>81</v>
       </c>
       <c r="C52" s="29"/>
-      <c r="D52" s="204"/>
-      <c r="E52" s="205"/>
+      <c r="D52" s="252"/>
+      <c r="E52" s="249"/>
       <c r="F52" s="6"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
@@ -4800,15 +4791,15 @@
         <v>82</v>
       </c>
       <c r="C53" s="29"/>
-      <c r="D53" s="206" t="str">
+      <c r="D53" s="250" t="str">
         <f>IF(F52="","_empty_",F52)</f>
         <v>_empty_</v>
       </c>
-      <c r="E53" s="207"/>
-      <c r="F53" s="208" t="s">
+      <c r="E53" s="251"/>
+      <c r="F53" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="G53" s="209"/>
+      <c r="G53" s="247"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="J53" s="2"/>
@@ -4844,8 +4835,8 @@
         <v>83</v>
       </c>
       <c r="C54" s="29"/>
-      <c r="D54" s="204"/>
-      <c r="E54" s="205"/>
+      <c r="D54" s="252"/>
+      <c r="E54" s="249"/>
       <c r="F54" s="6"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
@@ -4883,15 +4874,15 @@
         <v>84</v>
       </c>
       <c r="C55" s="29"/>
-      <c r="D55" s="206" t="str">
+      <c r="D55" s="250" t="str">
         <f>IF(F54="","_empty_",F54)</f>
         <v>_empty_</v>
       </c>
-      <c r="E55" s="207"/>
-      <c r="F55" s="208" t="s">
+      <c r="E55" s="251"/>
+      <c r="F55" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="G55" s="209"/>
+      <c r="G55" s="247"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="2"/>
@@ -4927,8 +4918,8 @@
         <v>85</v>
       </c>
       <c r="C56" s="29"/>
-      <c r="D56" s="204"/>
-      <c r="E56" s="205"/>
+      <c r="D56" s="252"/>
+      <c r="E56" s="249"/>
       <c r="F56" s="6"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
@@ -4966,15 +4957,15 @@
         <v>86</v>
       </c>
       <c r="C57" s="29"/>
-      <c r="D57" s="206" t="str">
+      <c r="D57" s="250" t="str">
         <f>IF(F56="","_empty_",F56)</f>
         <v>_empty_</v>
       </c>
-      <c r="E57" s="207"/>
-      <c r="F57" s="208" t="s">
+      <c r="E57" s="251"/>
+      <c r="F57" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="G57" s="209"/>
+      <c r="G57" s="247"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="J57" s="2"/>
@@ -5010,8 +5001,8 @@
         <v>87</v>
       </c>
       <c r="C58" s="29"/>
-      <c r="D58" s="204"/>
-      <c r="E58" s="205"/>
+      <c r="D58" s="252"/>
+      <c r="E58" s="249"/>
       <c r="F58" s="6"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
@@ -5049,15 +5040,15 @@
         <v>88</v>
       </c>
       <c r="C59" s="29"/>
-      <c r="D59" s="206" t="str">
+      <c r="D59" s="250" t="str">
         <f>IF(F58="","_empty_",F58)</f>
         <v>_empty_</v>
       </c>
-      <c r="E59" s="207"/>
-      <c r="F59" s="208" t="s">
+      <c r="E59" s="251"/>
+      <c r="F59" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="G59" s="209"/>
+      <c r="G59" s="247"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
       <c r="J59" s="2"/>
@@ -5093,8 +5084,8 @@
         <v>89</v>
       </c>
       <c r="C60" s="29"/>
-      <c r="D60" s="204"/>
-      <c r="E60" s="205"/>
+      <c r="D60" s="252"/>
+      <c r="E60" s="249"/>
       <c r="F60" s="6"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
@@ -5132,15 +5123,15 @@
         <v>90</v>
       </c>
       <c r="C61" s="29"/>
-      <c r="D61" s="206" t="str">
+      <c r="D61" s="250" t="str">
         <f>IF(F60="","_empty_",F60)</f>
         <v>_empty_</v>
       </c>
-      <c r="E61" s="207"/>
-      <c r="F61" s="208" t="s">
+      <c r="E61" s="251"/>
+      <c r="F61" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="G61" s="209"/>
+      <c r="G61" s="247"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="2"/>
@@ -5176,8 +5167,8 @@
         <v>91</v>
       </c>
       <c r="C62" s="29"/>
-      <c r="D62" s="204"/>
-      <c r="E62" s="205"/>
+      <c r="D62" s="252"/>
+      <c r="E62" s="249"/>
       <c r="F62" s="6"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
@@ -5215,15 +5206,15 @@
         <v>92</v>
       </c>
       <c r="C63" s="29"/>
-      <c r="D63" s="206" t="str">
+      <c r="D63" s="250" t="str">
         <f>IF(F62="","_empty_",F62)</f>
         <v>_empty_</v>
       </c>
-      <c r="E63" s="207"/>
-      <c r="F63" s="208" t="s">
+      <c r="E63" s="251"/>
+      <c r="F63" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="G63" s="209"/>
+      <c r="G63" s="247"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
       <c r="J63" s="2"/>
@@ -5259,8 +5250,8 @@
         <v>93</v>
       </c>
       <c r="C64" s="29"/>
-      <c r="D64" s="204"/>
-      <c r="E64" s="205"/>
+      <c r="D64" s="252"/>
+      <c r="E64" s="249"/>
       <c r="F64" s="6"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
@@ -5298,15 +5289,15 @@
         <v>94</v>
       </c>
       <c r="C65" s="29"/>
-      <c r="D65" s="206" t="str">
+      <c r="D65" s="250" t="str">
         <f>IF(F64="","_empty_",F64)</f>
         <v>_empty_</v>
       </c>
-      <c r="E65" s="207"/>
-      <c r="F65" s="208" t="s">
+      <c r="E65" s="251"/>
+      <c r="F65" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="G65" s="209"/>
+      <c r="G65" s="247"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="J65" s="2"/>
@@ -5342,8 +5333,8 @@
         <v>95</v>
       </c>
       <c r="C66" s="29"/>
-      <c r="D66" s="204"/>
-      <c r="E66" s="205"/>
+      <c r="D66" s="252"/>
+      <c r="E66" s="249"/>
       <c r="F66" s="6"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
@@ -5381,15 +5372,15 @@
         <v>96</v>
       </c>
       <c r="C67" s="29"/>
-      <c r="D67" s="206" t="str">
+      <c r="D67" s="250" t="str">
         <f>IF(F66="","_empty_",F66)</f>
         <v>_empty_</v>
       </c>
-      <c r="E67" s="207"/>
-      <c r="F67" s="208" t="s">
+      <c r="E67" s="251"/>
+      <c r="F67" s="246" t="s">
         <v>74</v>
       </c>
-      <c r="G67" s="209"/>
+      <c r="G67" s="247"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="J67" s="2"/>
@@ -5421,14 +5412,14 @@
       </c>
     </row>
     <row r="68" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B68" s="202" t="s">
+      <c r="B68" s="253" t="s">
         <v>97</v>
       </c>
-      <c r="C68" s="203"/>
-      <c r="D68" s="203"/>
-      <c r="E68" s="203"/>
-      <c r="F68" s="203"/>
-      <c r="G68" s="203"/>
+      <c r="C68" s="254"/>
+      <c r="D68" s="254"/>
+      <c r="E68" s="254"/>
+      <c r="F68" s="254"/>
+      <c r="G68" s="254"/>
       <c r="H68" s="1">
         <f t="shared" ref="H68:O68" si="5">SUM(H45:H67)</f>
         <v>0</v>
@@ -5464,15 +5455,15 @@
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25"/>
     <row r="70" spans="2:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B70" s="190" t="s">
+      <c r="B70" s="255" t="s">
         <v>98</v>
       </c>
-      <c r="C70" s="191"/>
-      <c r="D70" s="191"/>
-      <c r="E70" s="191"/>
-      <c r="F70" s="191"/>
-      <c r="G70" s="192"/>
-      <c r="H70" s="192"/>
+      <c r="C70" s="256"/>
+      <c r="D70" s="256"/>
+      <c r="E70" s="256"/>
+      <c r="F70" s="256"/>
+      <c r="G70" s="257"/>
+      <c r="H70" s="257"/>
       <c r="I70" s="34" t="s">
         <v>10</v>
       </c>
@@ -5512,8 +5503,8 @@
       <c r="D72" s="97"/>
       <c r="E72" s="97"/>
       <c r="F72" s="97"/>
-      <c r="G72" s="193"/>
-      <c r="H72" s="194"/>
+      <c r="G72" s="258"/>
+      <c r="H72" s="259"/>
       <c r="I72" s="98" t="s">
         <v>101</v>
       </c>
@@ -5532,8 +5523,8 @@
       <c r="D73" s="102"/>
       <c r="E73" s="102"/>
       <c r="F73" s="102"/>
-      <c r="G73" s="195"/>
-      <c r="H73" s="196"/>
+      <c r="G73" s="260"/>
+      <c r="H73" s="261"/>
       <c r="I73" s="103" t="s">
         <v>103</v>
       </c>
@@ -5545,15 +5536,15 @@
       <c r="O73" s="104"/>
     </row>
     <row r="74" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B74" s="197" t="s">
+      <c r="B74" s="262" t="s">
         <v>104</v>
       </c>
-      <c r="C74" s="198"/>
-      <c r="D74" s="199"/>
-      <c r="E74" s="199"/>
-      <c r="F74" s="199"/>
-      <c r="G74" s="200"/>
-      <c r="H74" s="201"/>
+      <c r="C74" s="263"/>
+      <c r="D74" s="264"/>
+      <c r="E74" s="264"/>
+      <c r="F74" s="264"/>
+      <c r="G74" s="265"/>
+      <c r="H74" s="266"/>
       <c r="I74" s="105" t="s">
         <v>105</v>
       </c>
@@ -5572,15 +5563,15 @@
       <c r="D75" s="109"/>
       <c r="E75" s="109"/>
       <c r="F75" s="108"/>
-      <c r="G75" s="184"/>
-      <c r="H75" s="185"/>
-      <c r="I75" s="185"/>
-      <c r="J75" s="185"/>
-      <c r="K75" s="185"/>
-      <c r="L75" s="185"/>
-      <c r="M75" s="185"/>
-      <c r="N75" s="185"/>
-      <c r="O75" s="186"/>
+      <c r="G75" s="268"/>
+      <c r="H75" s="269"/>
+      <c r="I75" s="269"/>
+      <c r="J75" s="269"/>
+      <c r="K75" s="269"/>
+      <c r="L75" s="269"/>
+      <c r="M75" s="269"/>
+      <c r="N75" s="269"/>
+      <c r="O75" s="270"/>
     </row>
     <row r="76" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="110"/>
@@ -5652,16 +5643,16 @@
       <c r="G79" s="127" t="s">
         <v>111</v>
       </c>
-      <c r="H79" s="187" t="s">
+      <c r="H79" s="271" t="s">
         <v>112</v>
       </c>
-      <c r="I79" s="187"/>
-      <c r="J79" s="187"/>
-      <c r="K79" s="187"/>
-      <c r="L79" s="187"/>
-      <c r="M79" s="187"/>
-      <c r="N79" s="187"/>
-      <c r="O79" s="188"/>
+      <c r="I79" s="271"/>
+      <c r="J79" s="271"/>
+      <c r="K79" s="271"/>
+      <c r="L79" s="271"/>
+      <c r="M79" s="271"/>
+      <c r="N79" s="271"/>
+      <c r="O79" s="272"/>
     </row>
     <row r="80" spans="2:26" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="123" t="s">
@@ -5677,16 +5668,16 @@
       <c r="G80" s="127" t="s">
         <v>111</v>
       </c>
-      <c r="H80" s="187" t="s">
+      <c r="H80" s="271" t="s">
         <v>114</v>
       </c>
-      <c r="I80" s="187"/>
-      <c r="J80" s="187"/>
-      <c r="K80" s="187"/>
-      <c r="L80" s="187"/>
-      <c r="M80" s="187"/>
-      <c r="N80" s="187"/>
-      <c r="O80" s="188"/>
+      <c r="I80" s="271"/>
+      <c r="J80" s="271"/>
+      <c r="K80" s="271"/>
+      <c r="L80" s="271"/>
+      <c r="M80" s="271"/>
+      <c r="N80" s="271"/>
+      <c r="O80" s="272"/>
     </row>
     <row r="81" spans="2:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="123" t="s">
@@ -5702,16 +5693,16 @@
       <c r="G81" s="127" t="s">
         <v>111</v>
       </c>
-      <c r="H81" s="187" t="s">
+      <c r="H81" s="271" t="s">
         <v>116</v>
       </c>
-      <c r="I81" s="187"/>
-      <c r="J81" s="187"/>
-      <c r="K81" s="187"/>
-      <c r="L81" s="187"/>
-      <c r="M81" s="187"/>
-      <c r="N81" s="187"/>
-      <c r="O81" s="188"/>
+      <c r="I81" s="271"/>
+      <c r="J81" s="271"/>
+      <c r="K81" s="271"/>
+      <c r="L81" s="271"/>
+      <c r="M81" s="271"/>
+      <c r="N81" s="271"/>
+      <c r="O81" s="272"/>
     </row>
     <row r="82" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B82" s="128" t="s">
@@ -5893,7 +5884,7 @@
       </c>
     </row>
     <row r="91" spans="2:15" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E91" s="189" t="s">
+      <c r="E91" s="273" t="s">
         <v>141</v>
       </c>
       <c r="F91" s="154" t="s">
@@ -5911,7 +5902,7 @@
       </c>
     </row>
     <row r="92" spans="2:15" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E92" s="189"/>
+      <c r="E92" s="273"/>
       <c r="F92" s="158" t="s">
         <v>144</v>
       </c>
@@ -5927,7 +5918,7 @@
       </c>
     </row>
     <row r="93" spans="2:15" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E93" s="189"/>
+      <c r="E93" s="273"/>
       <c r="F93" s="154" t="s">
         <v>146</v>
       </c>
@@ -5943,7 +5934,7 @@
       </c>
     </row>
     <row r="94" spans="2:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E94" s="189"/>
+      <c r="E94" s="273"/>
       <c r="F94" s="158" t="s">
         <v>148</v>
       </c>
@@ -5957,7 +5948,7 @@
       </c>
     </row>
     <row r="95" spans="2:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E95" s="189"/>
+      <c r="E95" s="273"/>
       <c r="F95" s="163" t="s">
         <v>149</v>
       </c>
@@ -5973,7 +5964,7 @@
       </c>
     </row>
     <row r="96" spans="2:15" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E96" s="189"/>
+      <c r="E96" s="273"/>
       <c r="F96" s="167" t="s">
         <v>149</v>
       </c>
@@ -5989,7 +5980,7 @@
       </c>
     </row>
     <row r="97" spans="5:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E97" s="189"/>
+      <c r="E97" s="273"/>
       <c r="F97" s="154" t="s">
         <v>154</v>
       </c>
@@ -6003,7 +5994,7 @@
       </c>
     </row>
     <row r="98" spans="5:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E98" s="189"/>
+      <c r="E98" s="273"/>
       <c r="F98" s="158" t="s">
         <v>155</v>
       </c>
@@ -6017,7 +6008,7 @@
       </c>
     </row>
     <row r="99" spans="5:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E99" s="183" t="s">
+      <c r="E99" s="267" t="s">
         <v>156</v>
       </c>
       <c r="F99" s="154" t="s">
@@ -6035,7 +6026,7 @@
       </c>
     </row>
     <row r="100" spans="5:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E100" s="183"/>
+      <c r="E100" s="267"/>
       <c r="F100" s="169" t="s">
         <v>159</v>
       </c>
@@ -6048,7 +6039,7 @@
       </c>
     </row>
     <row r="101" spans="5:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E101" s="183"/>
+      <c r="E101" s="267"/>
       <c r="F101" s="154" t="s">
         <v>160</v>
       </c>
@@ -6064,7 +6055,7 @@
       </c>
     </row>
     <row r="102" spans="5:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E102" s="183"/>
+      <c r="E102" s="267"/>
       <c r="F102" s="173" t="s">
         <v>162</v>
       </c>
@@ -6077,7 +6068,7 @@
       </c>
     </row>
     <row r="103" spans="5:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E103" s="183"/>
+      <c r="E103" s="267"/>
       <c r="F103" s="154" t="s">
         <v>163</v>
       </c>
@@ -6090,7 +6081,7 @@
       </c>
     </row>
     <row r="104" spans="5:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E104" s="183"/>
+      <c r="E104" s="267"/>
       <c r="F104" s="178" t="s">
         <v>154</v>
       </c>
@@ -6103,7 +6094,7 @@
       </c>
     </row>
     <row r="105" spans="5:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E105" s="183"/>
+      <c r="E105" s="267"/>
       <c r="F105" s="154" t="s">
         <v>164</v>
       </c>
@@ -6116,7 +6107,7 @@
       </c>
     </row>
     <row r="106" spans="5:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E106" s="183"/>
+      <c r="E106" s="267"/>
       <c r="F106" s="178" t="s">
         <v>166</v>
       </c>
@@ -6130,7 +6121,7 @@
       <c r="J106" s="19"/>
     </row>
     <row r="107" spans="5:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E107" s="183"/>
+      <c r="E107" s="267"/>
       <c r="F107" s="154" t="s">
         <v>167</v>
       </c>
@@ -6144,7 +6135,7 @@
       <c r="J107" s="19"/>
     </row>
     <row r="108" spans="5:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E108" s="183"/>
+      <c r="E108" s="267"/>
       <c r="F108" s="178" t="s">
         <v>168</v>
       </c>
@@ -6158,7 +6149,7 @@
       <c r="J108" s="19"/>
     </row>
     <row r="109" spans="5:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E109" s="183"/>
+      <c r="E109" s="267"/>
       <c r="F109" s="154" t="s">
         <v>169</v>
       </c>
@@ -6172,7 +6163,7 @@
       <c r="J109" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection sheet="1" selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="F34" name="Orange fields_1"/>
     <protectedRange sqref="G41:N41" name="Orange fields_3"/>
@@ -6180,36 +6171,53 @@
     <protectedRange sqref="H75 G72:G74" name="Orange fields_2"/>
   </protectedRanges>
   <mergeCells count="93">
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="I38:O38"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="I34:O35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="I36:O37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="B27:O27"/>
-    <mergeCell ref="I29:O29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="I30:O30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="I31:O31"/>
-    <mergeCell ref="B15:O15"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I20:O20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H3:O3"/>
-    <mergeCell ref="H4:O4"/>
-    <mergeCell ref="H5:O5"/>
-    <mergeCell ref="H6:O6"/>
-    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="E99:E109"/>
+    <mergeCell ref="G75:O75"/>
+    <mergeCell ref="H79:O79"/>
+    <mergeCell ref="H80:O80"/>
+    <mergeCell ref="H81:O81"/>
+    <mergeCell ref="E91:E98"/>
+    <mergeCell ref="B70:H70"/>
+    <mergeCell ref="G72:H72"/>
+    <mergeCell ref="G73:H73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="G74:H74"/>
+    <mergeCell ref="B68:G68"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
     <mergeCell ref="B41:O41"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="D43:E43"/>
@@ -6226,53 +6234,36 @@
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="I26:O26"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="B68:G68"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="B70:H70"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="G74:H74"/>
-    <mergeCell ref="E99:E109"/>
-    <mergeCell ref="G75:O75"/>
-    <mergeCell ref="H79:O79"/>
-    <mergeCell ref="H80:O80"/>
-    <mergeCell ref="H81:O81"/>
-    <mergeCell ref="E91:E98"/>
+    <mergeCell ref="H3:O3"/>
+    <mergeCell ref="H4:O4"/>
+    <mergeCell ref="H5:O5"/>
+    <mergeCell ref="H6:O6"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="B15:O15"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I20:O20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="B27:O27"/>
+    <mergeCell ref="I29:O29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="I30:O30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="I31:O31"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="I38:O38"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="I34:O35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="I36:O37"/>
+    <mergeCell ref="F37:G37"/>
   </mergeCells>
   <conditionalFormatting sqref="D45:E67">
     <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="_empty_">

</xml_diff>